<commit_message>
Updated experiment result with new k for cross-validation
</commit_message>
<xml_diff>
--- a/Parameters-Estimation/Ck_Parameters_Estimation/1-Trained-Models/training_2016_2017_test_2018_2019_comparing_old_model/Results-ck-calibration-model-k-10-old-configuration.xlsx
+++ b/Parameters-Estimation/Ck_Parameters_Estimation/1-Trained-Models/training_2016_2017_test_2018_2019_comparing_old_model/Results-ck-calibration-model-k-10-old-configuration.xlsx
@@ -13,7 +13,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>random_forest</t>
+  </si>
+  <si>
+    <t>lsboost</t>
+  </si>
+  <si>
+    <t>neural_network</t>
+  </si>
+  <si>
+    <t>old_model</t>
+  </si>
+  <si>
+    <t>RMSE</t>
+  </si>
+  <si>
+    <t>NRMSE</t>
+  </si>
+  <si>
+    <t>MAE</t>
+  </si>
+  <si>
+    <t>RSE</t>
+  </si>
+  <si>
+    <t>RRSE</t>
+  </si>
+  <si>
+    <t>RAE</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>Corr Coeff</t>
+  </si>
   <si>
     <t>Row</t>
   </si>
@@ -152,123 +191,123 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B2" s="0">
-        <v>56.279652029263914</v>
+        <v>57.080564413808737</v>
       </c>
       <c r="C2" s="0">
-        <v>0.42695547995769617</v>
+        <v>0.43303145802823562</v>
       </c>
       <c r="D2" s="0">
-        <v>39.579939524996234</v>
+        <v>40.29733989091374</v>
       </c>
       <c r="E2" s="0">
-        <v>0.47183022909002914</v>
+        <v>0.48535495991138794</v>
       </c>
       <c r="F2" s="0">
-        <v>0.68689899482385997</v>
+        <v>0.69667421361163351</v>
       </c>
       <c r="G2" s="0">
-        <v>0.6666845240549103</v>
+        <v>0.67876841622979556</v>
       </c>
       <c r="H2" s="0">
-        <v>0.52816977090997086</v>
+        <v>0.514645040088612</v>
       </c>
       <c r="I2" s="0">
-        <v>0.72969421515559363</v>
+        <v>0.71950071203295229</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B3" s="0">
-        <v>57.662872250677879</v>
+        <v>57.507675829328143</v>
       </c>
       <c r="C3" s="0">
-        <v>0.43744903192944445</v>
+        <v>0.43627166213101998</v>
       </c>
       <c r="D3" s="0">
-        <v>40.289747913648419</v>
+        <v>39.87109185972411</v>
       </c>
       <c r="E3" s="0">
-        <v>0.49530817622683865</v>
+        <v>0.4926455752264578</v>
       </c>
       <c r="F3" s="0">
-        <v>0.70378134120395563</v>
+        <v>0.70188715277205194</v>
       </c>
       <c r="G3" s="0">
-        <v>0.67864053696038507</v>
+        <v>0.67158869414801881</v>
       </c>
       <c r="H3" s="0">
-        <v>0.50469182377316135</v>
+        <v>0.5073544247735422</v>
       </c>
       <c r="I3" s="0">
-        <v>0.7125625768781807</v>
+        <v>0.7125290597160111</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B4" s="0">
-        <v>58.894870422016176</v>
+        <v>62.510332793576197</v>
       </c>
       <c r="C4" s="0">
-        <v>0.44679536495718308</v>
+        <v>0.47422342139427237</v>
       </c>
       <c r="D4" s="0">
-        <v>41.16213889211209</v>
+        <v>44.817700701314081</v>
       </c>
       <c r="E4" s="0">
-        <v>0.51669932685116882</v>
+        <v>0.58208522606355118</v>
       </c>
       <c r="F4" s="0">
-        <v>0.71881800676608598</v>
+        <v>0.76294510029460916</v>
       </c>
       <c r="G4" s="0">
-        <v>0.6933350911018723</v>
+        <v>0.75490937631223787</v>
       </c>
       <c r="H4" s="0">
-        <v>0.48330067314883118</v>
+        <v>0.41791477393644882</v>
       </c>
       <c r="I4" s="0">
-        <v>0.70031184160794491</v>
+        <v>0.65313901048550294</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B5" s="0">
         <v>79.31940644599392</v>

</xml_diff>